<commit_message>
add Nordic rating to Evans2010 pole list
</commit_message>
<xml_diff>
--- a/Data/Evans2010_Superior_poles.xlsx
+++ b/Data/Evans2010_Superior_poles.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Laurentia/Google Drive/Service_Outreach/Hodgkiss_Quals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/superior/0000_Github/Laurentia_Paleogeography/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC97CEE0-4587-8242-906E-1D9728981EAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D173FE32-CAD5-B142-97B5-CD5321D92E98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24480" yWindow="4580" windowWidth="27640" windowHeight="16940" xr2:uid="{ADDB269D-EE8E-B74F-8362-56B8A4D5CF88}"/>
+    <workbookView xWindow="2780" yWindow="2920" windowWidth="28800" windowHeight="16320" xr2:uid="{ADDB269D-EE8E-B74F-8362-56B8A4D5CF88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Otto Stock lamproph.</t>
   </si>
@@ -497,6 +503,15 @@
       </rPr>
       <t>Halls and Heaman (2000); recalc. Evans and Halls (2010) (W)</t>
     </r>
+  </si>
+  <si>
+    <t>Leirubakki_rating</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -893,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4E0725-58E4-F148-AE58-B4175D6E7FAE}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,7 +921,7 @@
     <col min="11" max="11" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -940,8 +955,11 @@
       <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,8 +993,11 @@
       <c r="K2" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="L2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -1010,8 +1031,11 @@
       <c r="K3" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1046,8 +1070,11 @@
       <c r="K4" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="L4" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1081,8 +1108,11 @@
       <c r="K5" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="L5" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1116,8 +1146,11 @@
       <c r="K6" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1151,8 +1184,11 @@
       <c r="K7" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="L7" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1186,8 +1222,11 @@
       <c r="K8" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L8" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -1222,8 +1261,11 @@
       <c r="K9" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="L9" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -1258,8 +1300,11 @@
       <c r="K10" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="L10" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1293,8 +1338,11 @@
       <c r="K11" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="L11" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1328,8 +1376,11 @@
       <c r="K12" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="L12" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1363,8 +1414,11 @@
       <c r="K13" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="L13" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1398,8 +1452,11 @@
       <c r="K14" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="L14" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
@@ -1433,8 +1490,11 @@
       <c r="K15" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="L15" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>